<commit_message>
#207 Some update to CS Data
</commit_message>
<xml_diff>
--- a/Files/data/Processed Data/Tabelas/CS Grids - 2019.1-2024.1.xlsx
+++ b/Files/data/Processed Data/Tabelas/CS Grids - 2019.1-2024.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\timetabling-UENF\Files\data\Processed Data\Tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458F4F38-0B3E-4334-8C82-57459343F17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BCA86B-31BF-4607-B65F-ABCA8F7A9205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="24.1-v0" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="23.1-v8" sheetId="3" r:id="rId3"/>
     <sheet name="22.2-v5" sheetId="4" r:id="rId4"/>
     <sheet name="22.1-v3.4" sheetId="5" r:id="rId5"/>
-    <sheet name="X21.2" sheetId="6" r:id="rId6"/>
-    <sheet name="X21.1" sheetId="7" r:id="rId7"/>
-    <sheet name="X20.2" sheetId="8" r:id="rId8"/>
-    <sheet name="20.1" sheetId="9" r:id="rId9"/>
-    <sheet name="19.2" sheetId="10" r:id="rId10"/>
-    <sheet name="19.1" sheetId="11" r:id="rId11"/>
+    <sheet name="21.2-X" sheetId="6" r:id="rId6"/>
+    <sheet name="21.1-X" sheetId="7" r:id="rId7"/>
+    <sheet name="20.2-X" sheetId="8" r:id="rId8"/>
+    <sheet name="20.1-v" sheetId="9" r:id="rId9"/>
+    <sheet name="19.2-v" sheetId="10" r:id="rId10"/>
+    <sheet name="19.1-v" sheetId="11" r:id="rId11"/>
     <sheet name="limpo" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -1000,8 +1000,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="20" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1011,9 +1021,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1025,26 +1032,19 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1353,12 +1353,12 @@
   </sheetPr>
   <dimension ref="A1:K144"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.33203125" style="9" bestFit="1" customWidth="1"/>
@@ -1366,11 +1366,12 @@
     <col min="4" max="5" width="36.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.5546875" hidden="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.5546875" hidden="1"/>
+    <col min="12" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
+      <c r="A1" s="16"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1388,185 +1389,185 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30">
+      <c r="A2" s="17">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="19" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30">
+      <c r="A3" s="17">
         <v>0.375</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30">
+      <c r="A4" s="17">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30">
+      <c r="A5" s="17">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
+      <c r="A6" s="17">
         <v>0.5</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30">
+      <c r="A7" s="17">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30">
+      <c r="A8" s="17">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="19" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30">
+      <c r="A9" s="17">
         <v>0.625</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30">
+      <c r="A10" s="17">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+      <c r="A11" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="A12" s="17">
         <v>0.75</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30">
+      <c r="A13" s="17">
         <v>0.79166666666666663</v>
       </c>
       <c r="B13" s="20"/>
-      <c r="C13" s="17"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="20"/>
-      <c r="E13" s="17"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="20"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
+      <c r="A14" s="16"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:6" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:6" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="15"/>
     </row>
     <row r="21" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -1753,36 +1754,36 @@
     <row r="144" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1793,7 +1794,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1813,7 +1814,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
+      <c r="A1" s="16"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1831,171 +1832,171 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30">
+      <c r="A2" s="17">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="29" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30">
+      <c r="A3" s="17">
         <v>0.375</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30">
+      <c r="A4" s="17">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="27" t="s">
         <v>37</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="29" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30">
+      <c r="A5" s="17">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="31" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="26"/>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
+      <c r="A6" s="17">
         <v>0.5</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30">
+      <c r="A7" s="17">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
     </row>
     <row r="8" spans="1:6" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30">
+      <c r="A8" s="17">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="27" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30">
+      <c r="A9" s="17">
         <v>0.625</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
     </row>
     <row r="10" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30">
+      <c r="A10" s="17">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="F10" s="26"/>
+      <c r="F10" s="27"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+      <c r="A11" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="A12" s="17">
         <v>0.75</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26" t="s">
+      <c r="C12" s="27"/>
+      <c r="D12" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30">
+      <c r="A13" s="17">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
+      <c r="A14" s="16"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3"/>
@@ -2003,21 +2004,11 @@
     <row r="18" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
@@ -2027,11 +2018,21 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2046,10 +2047,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8:C9"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
@@ -2057,10 +2058,12 @@
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
+      <c r="A1" s="16"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2078,208 +2081,208 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30">
+      <c r="A2" s="17">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="F2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30">
+      <c r="A3" s="17">
         <v>0.375</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30">
+      <c r="A4" s="17">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="29" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30">
+      <c r="A5" s="17">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
+      <c r="A6" s="17">
         <v>0.5</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26" t="s">
+      <c r="D6" s="27"/>
+      <c r="E6" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="26"/>
+      <c r="F6" s="27"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30">
+      <c r="A7" s="17">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
     </row>
     <row r="8" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30">
+      <c r="A8" s="17">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="29" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30">
+      <c r="A9" s="17">
         <v>0.625</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
     </row>
     <row r="10" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30">
+      <c r="A10" s="17">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="27" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+      <c r="A11" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="A12" s="17">
         <v>0.75</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30">
+      <c r="A13" s="17">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
+      <c r="A14" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2290,7 +2293,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2309,7 +2312,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
+      <c r="A1" s="16"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2327,160 +2330,160 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30">
+      <c r="A2" s="17">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30">
+      <c r="A3" s="17">
         <v>0.375</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30">
+      <c r="A4" s="17">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30">
+      <c r="A5" s="17">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
+      <c r="A6" s="17">
         <v>0.5</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30">
+      <c r="A7" s="17">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30">
+      <c r="A8" s="17">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30">
+      <c r="A9" s="17">
         <v>0.625</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30">
+      <c r="A10" s="17">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+      <c r="A11" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="A12" s="17">
         <v>0.75</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30">
+      <c r="A13" s="17">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
+      <c r="A14" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2491,23 +2494,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6:D7"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
+      <c r="A1" s="16"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2525,171 +2530,171 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30">
+      <c r="A2" s="17">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30">
+      <c r="A3" s="17">
         <v>0.375</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30">
+      <c r="A4" s="17">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="24" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30">
+      <c r="A5" s="17">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="17"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
+      <c r="A6" s="17">
         <v>0.5</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30">
+      <c r="A7" s="17">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30">
+      <c r="A8" s="17">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="24" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30">
+      <c r="A9" s="17">
         <v>0.625</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
     </row>
     <row r="10" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30">
+      <c r="A10" s="17">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+      <c r="A11" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
     </row>
     <row r="12" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="A12" s="17">
         <v>0.75</v>
       </c>
       <c r="B12" s="12"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21" t="s">
+      <c r="C12" s="24"/>
+      <c r="D12" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
     </row>
     <row r="13" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30">
+      <c r="A13" s="17">
         <v>0.79166666666666663</v>
       </c>
       <c r="B13" s="13"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="17"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="20"/>
     </row>
     <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
         <v>31</v>
       </c>
@@ -2697,18 +2702,23 @@
       <c r="D14" s="14"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3"/>
+    <row r="17" x14ac:dyDescent="0.3"/>
+    <row r="18" x14ac:dyDescent="0.3"/>
+    <row r="19" x14ac:dyDescent="0.3"/>
+    <row r="20" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
@@ -2717,16 +2727,16 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2737,14 +2747,14 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" style="9" bestFit="1" customWidth="1"/>
@@ -2752,10 +2762,12 @@
     <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
+      <c r="A1" s="16"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2773,202 +2785,208 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30">
+      <c r="A2" s="17">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="24" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30">
+      <c r="A3" s="17">
         <v>0.375</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
     </row>
     <row r="4" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30">
+      <c r="A4" s="17">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="24" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30">
+      <c r="A5" s="17">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
     </row>
     <row r="6" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
+      <c r="A6" s="17">
         <v>0.5</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30">
+      <c r="A7" s="17">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30">
+      <c r="A8" s="17">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="24" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30">
+      <c r="A9" s="17">
         <v>0.625</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
     </row>
     <row r="10" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30">
+      <c r="A10" s="17">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="24" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+      <c r="A11" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="22"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="25"/>
     </row>
     <row r="12" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="A12" s="17">
         <v>0.75</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
     </row>
     <row r="13" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30">
+      <c r="A13" s="17">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="17"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="20"/>
-      <c r="E13" s="17"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="20"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
-    </row>
+      <c r="A14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3"/>
+    <row r="17" x14ac:dyDescent="0.3"/>
+    <row r="18" x14ac:dyDescent="0.3"/>
+    <row r="19" x14ac:dyDescent="0.3"/>
+    <row r="20" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2979,14 +2997,14 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" style="9" bestFit="1" customWidth="1"/>
@@ -2994,10 +3012,12 @@
     <col min="4" max="4" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
+      <c r="A1" s="16"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3015,195 +3035,191 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30">
+      <c r="A2" s="17">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="19" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30">
+      <c r="A3" s="17">
         <v>0.375</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-    </row>
-    <row r="4" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="17">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="19" t="s">
         <v>111</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="19" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30">
+    <row r="5" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="F5" s="17"/>
-    </row>
-    <row r="6" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
+      <c r="F5" s="21"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="17">
         <v>0.5</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="18"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30">
+      <c r="A7" s="17">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="19"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30">
+      <c r="A8" s="17">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="19" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30">
+      <c r="A9" s="17">
         <v>0.625</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30">
+      <c r="A10" s="17">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="19" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+      <c r="A11" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="A12" s="17">
         <v>0.75</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="F12" s="16"/>
+      <c r="F12" s="19"/>
     </row>
     <row r="13" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30">
+      <c r="A13" s="17">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
-    </row>
+      <c r="A14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3"/>
+    <row r="17" x14ac:dyDescent="0.3"/>
+    <row r="18" x14ac:dyDescent="0.3"/>
+    <row r="19" x14ac:dyDescent="0.3"/>
+    <row r="20" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
@@ -3212,11 +3228,21 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3227,24 +3253,26 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <pane ySplit="1" topLeftCell="A1048550" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
+      <c r="A1" s="16"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3262,210 +3290,215 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30">
+      <c r="A2" s="17">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="29" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30">
+      <c r="A3" s="17">
         <v>0.375</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:6" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30">
+      <c r="A4" s="17">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="29" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30">
+      <c r="A5" s="17">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
+      <c r="A6" s="17">
         <v>0.5</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30">
+      <c r="A7" s="17">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
     </row>
     <row r="8" spans="1:6" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30">
+      <c r="A8" s="17">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="29" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30">
+      <c r="A9" s="17">
         <v>0.625</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
     </row>
     <row r="10" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30">
+      <c r="A10" s="17">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="29" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+      <c r="A11" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="A12" s="17">
         <v>0.75</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="27" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30">
+      <c r="A13" s="17">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
-    </row>
+      <c r="A14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3"/>
+    <row r="17" x14ac:dyDescent="0.3"/>
+    <row r="18" x14ac:dyDescent="0.3"/>
+    <row r="19" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3480,10 +3513,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
@@ -3491,10 +3524,12 @@
     <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
+      <c r="A1" s="16"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3512,160 +3547,160 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30">
+      <c r="A2" s="17">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30">
+      <c r="A3" s="17">
         <v>0.375</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30">
+      <c r="A4" s="17">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30">
+      <c r="A5" s="17">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
+      <c r="A6" s="17">
         <v>0.5</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30">
+      <c r="A7" s="17">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30">
+      <c r="A8" s="17">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30">
+      <c r="A9" s="17">
         <v>0.625</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30">
+      <c r="A10" s="17">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+      <c r="A11" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="A12" s="17">
         <v>0.75</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30">
+      <c r="A13" s="17">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
+      <c r="A14" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3680,20 +3715,22 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
+      <c r="A1" s="16"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3711,160 +3748,160 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30">
+      <c r="A2" s="17">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30">
+      <c r="A3" s="17">
         <v>0.375</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30">
+      <c r="A4" s="17">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30">
+      <c r="A5" s="17">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
+      <c r="A6" s="17">
         <v>0.5</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30">
+      <c r="A7" s="17">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30">
+      <c r="A8" s="17">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30">
+      <c r="A9" s="17">
         <v>0.625</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30">
+      <c r="A10" s="17">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+      <c r="A11" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="A12" s="17">
         <v>0.75</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30">
+      <c r="A13" s="17">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
+      <c r="A14" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3879,10 +3916,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
@@ -3890,10 +3927,12 @@
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
+      <c r="A1" s="16"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3911,160 +3950,160 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30">
+      <c r="A2" s="17">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30">
+      <c r="A3" s="17">
         <v>0.375</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30">
+      <c r="A4" s="17">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30">
+      <c r="A5" s="17">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
+      <c r="A6" s="17">
         <v>0.5</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30">
+      <c r="A7" s="17">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30">
+      <c r="A8" s="17">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30">
+      <c r="A9" s="17">
         <v>0.625</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30">
+      <c r="A10" s="17">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+      <c r="A11" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="A12" s="17">
         <v>0.75</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30">
+      <c r="A13" s="17">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
+      <c r="A14" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4075,7 +4114,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4095,7 +4134,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
+      <c r="A1" s="16"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4113,206 +4152,206 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30">
+      <c r="A2" s="17">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="27" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30">
+      <c r="A3" s="17">
         <v>0.375</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30">
+      <c r="A4" s="17">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="27" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30">
+      <c r="A5" s="17">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
+      <c r="A6" s="17">
         <v>0.5</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30">
+      <c r="A7" s="17">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
     </row>
     <row r="8" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="30">
+      <c r="A8" s="17">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="29" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30">
+      <c r="A9" s="17">
         <v>0.625</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
     </row>
     <row r="10" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30">
+      <c r="A10" s="17">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="29" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
+      <c r="A11" s="17">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
+      <c r="A12" s="17">
         <v>0.75</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30">
+      <c r="A13" s="17">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
+      <c r="A14" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
#207 Last adjustments to insert data, but dropping out
I'll need to process it even more, and I don't want to.
</commit_message>
<xml_diff>
--- a/Files/data/Processed Data/Tabelas/CS Grids - 2019.1-2024.1.xlsx
+++ b/Files/data/Processed Data/Tabelas/CS Grids - 2019.1-2024.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\timetabling-UENF\Files\data\Processed Data\Tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E479750-3520-41EF-B694-04EACB6A9A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219054DE-62FF-49FB-89F6-FDAA383E0059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="704" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="167">
   <si>
     <t>SEG</t>
   </si>
@@ -46,10 +46,6 @@
   </si>
   <si>
     <t>SEX</t>
-  </si>
-  <si>
-    <t>1|Inglês Instrumental I
-10|Monografia|Tang|Inf1</t>
   </si>
   <si>
     <t>1|Prog I|Annabell|27|Bcct
@@ -112,10 +108,6 @@
   </si>
   <si>
     <t>3|Arquitetura|Átila</t>
-  </si>
-  <si>
-    <t>2|Calculo Dif e Int 2|Eng e Comp
-4|Calculo III|Oscar</t>
   </si>
   <si>
     <t>1|Inglês Instrumental I
@@ -155,24 +147,6 @@
     <t>3|Est Dados I|Tang|25|Bcct
 5|Redes de Comp|João|30|sala
 9|Algoritmos em Grafos|L Mariano||Inf1</t>
-  </si>
-  <si>
-    <t>1|Lógica Mat|Tang|30|
-3|Método Mat|Beggio|25|
-2|Fisica I|||B
-3|Fisica II|||A
-3|Fisica Experimental II|||C
-7|Sistemas Distribuidos|João|6|Inf1</t>
-  </si>
-  <si>
-    <t>3|Fisica Experimental II|||A
-5|BD I|L Mariano|27|||B cct
-7|Teste Software||Inf1</t>
-  </si>
-  <si>
-    <t>1|Geo Analit|Elba|35|
-5|Eng Software|Ausb|28|B cct
-7|Proc Imagens|Rivera|5|inf1</t>
   </si>
   <si>
     <t>1|Org Comp|Bolsista|27
@@ -188,11 +162,6 @@
 7|Sistemas Distribuidos|João|6|Inf1</t>
   </si>
   <si>
-    <t>3|Fisica II||5||C
-5|BD I|L Mariano|27|B cct
-7|Teste Software|||Inf1</t>
-  </si>
-  <si>
     <t>1|Calculo I
 3|Calculo III|Oscar|15
 5|P Estocáticos|Guill|10|Inf2</t>
@@ -203,11 +172,6 @@
 7|Proc Imagens|Rivera|5|inf1</t>
   </si>
   <si>
-    <t>1|Prog I|Annabell|27|B cct
-7|Metodologia|Molina
-9|Algoritmos em Grafos|L Mariano||Inf1</t>
-  </si>
-  <si>
     <t>1|Calculo I
 3|Arquitet C|Bolsista|30</t>
   </si>
@@ -222,11 +186,6 @@
     <t>4|Calc Numérico|Oscar||108cct
 6|Pesq Operacional|Tang||Inf1
 8|Prog Concorrente|L Mariano</t>
-  </si>
-  <si>
-    <t>2|Fisica 1||106 e 109B|A e B
-6|Int Comp Grafica|Rivera||Inf2
-8|Comp Ambiental|Eduardo</t>
   </si>
   <si>
     <t>2|Calculo II|Rigoberto||106cct
@@ -283,10 +242,6 @@
 6|Compiladores|||Inf1</t>
   </si>
   <si>
-    <t>2|Inglês Instrumental II|||B
-5|Comp e Socied||23|107</t>
-  </si>
-  <si>
     <t>1|Calculo I|||106cct
 2|Inglês Instrumental II||||B
 4|Int Prob Estatístic||10|107</t>
@@ -307,12 +262,6 @@
     <t>1|Lógica Mat|Tang|40|207P3
 3|Arquitet C|Sanya|45|106P3
 7|Segurança Com|Ausb|10|inf2</t>
-  </si>
-  <si>
-    <t>1|Org Comp|Sanya|35|205E1
-3|Est Dados I|Tang|45|106P3
-5|L Formais|Annabell|10|inf1
-7|Teste Software|João|8|inf1</t>
   </si>
   <si>
     <t>3|Método Mat|Beggio|13|106P3
@@ -343,11 +292,6 @@
 7|Proc Imagens|Rivera|5|inf1</t>
   </si>
   <si>
-    <t>3|Est Dados I CC1|Tang|16|inf2
-5|BD I|L Mariano|13|inf1
-7|Metodologia|Molina|105P3</t>
-  </si>
-  <si>
     <t>1|Prog I|L Mariano|25|P3|B_R
 3|Est Dados I|Tang|45|106P3
 5|L Formais|Annabell|10|inf1
@@ -364,10 +308,6 @@
 5|P Estocáticos|Guillermo|11</t>
   </si>
   <si>
-    <t>1|Org Comp|Sanya|35|205E1
-8|Empreendedorismo|||109A</t>
-  </si>
-  <si>
     <t>3|Fisica Experimental II||||C
 5|BD I|L Mariano|13|inf1
 7|Metodologia|Molina</t>
@@ -436,11 +376,6 @@
     <t>2|Lógica Digital|Sânya|35
 4|Calculo Numérico|Wilma|3
 8|Proc Imagens|Rivera|8</t>
-  </si>
-  <si>
-    <t>2|Fisica Geral I|21
-4|Sist Operacional|João|10
-6|Pesquisa Operacional|Tang|3</t>
   </si>
   <si>
     <t>2|Est Discretas|Guillermo|40
@@ -499,11 +434,6 @@
     <t>2|Lab Fisica Geral I||15</t>
   </si>
   <si>
-    <t>1|Lógica Mat|Tang||AuditP5
-4|Cálc Núm|Elba||Apitão
-5|Redes de Comp||João</t>
-  </si>
-  <si>
     <t>2|Estruturas Discret|Oscar
 3|Método Mat|Beggio||Apitão
 5|Engenharia de Software
@@ -655,11 +585,6 @@
 8|Ger de Redes|Alvaro||Binf1</t>
   </si>
   <si>
-    <t>2|Lógica Digital|Átila||CCT 206
-4|Numérico|Eng e Comp
-6|lntelig Artificial|Anna||BInf1</t>
-  </si>
-  <si>
     <t>2|Programação 2|Riv||infCCT
 4|Prog Orient Objs|Anna||BInf1
 8|Top Microcontr|Átila||BInf2</t>
@@ -668,11 +593,6 @@
     <t>4|Prob e Estatistica||||mat*</t>
   </si>
   <si>
-    <t>2|Calculo Dif e Int 2|Eng e Comp
-4|Sis Operacional|João||BInf2
-6|Int Comp Grafica|Riv||BInf1</t>
-  </si>
-  <si>
     <t>4|Calculo III|Oscar
 6|Compiladores|João||BInf2
 8|Ger de Redes|Alvaro||Binf1</t>
@@ -691,16 +611,6 @@
     <t>2|Est Discretas|Oscar||CCT</t>
   </si>
   <si>
-    <t>2|Lógica Digital|Átila||CCT 206
-4|Cálc Numérico|Eng e Comp
-6|Intelig Artificial|Anna||BInf1</t>
-  </si>
-  <si>
-    <t>2|Calculo Dif e Int 2|Eng e Comp
-4|Sis Operacional|João||BInf2
-6|Int Comp Grafica</t>
-  </si>
-  <si>
     <t>6|Compiladores|João||BInf2</t>
   </si>
   <si>
@@ -711,11 +621,6 @@
   <si>
     <t>2|Programaçao 2|LM||infCCT
 10|Monografia|Tang||116p5</t>
-  </si>
-  <si>
-    <t>2|Programação 2|LM|infCCT
-9|Proj de Monografia|Riv||BInf1
-10|Estagio S|Ausb||116p5</t>
   </si>
   <si>
     <t>8|Sistemas Intel|Anna||BInf2</t>
@@ -757,11 +662,6 @@
 7|Interação Hom Maq|Riv||B2</t>
   </si>
   <si>
-    <t>3|Estrutura Dados 1|Tang|Sal 
-5|Engenharia de Soft|Ausb|B1 
-7|Metod Trab Cientif|||cct</t>
-  </si>
-  <si>
     <t>1|Calculo I|Mylane||106
 2|Calculo II|Oscar||107</t>
   </si>
@@ -781,11 +681,6 @@
 7|Sists Distrib|Antônio||B1</t>
   </si>
   <si>
-    <t>1|Organiz Comp|Luiz M|B2
-3|Calculo III|||206 207
-5|Proc Estocást|L Guill||205 E1</t>
-  </si>
-  <si>
     <t>3|Paradig Ling Prog|Ausb
 5|Banco Dados 1|Luiz M||B1
 9|Proc de Imagens|Riv||B2</t>
@@ -807,6 +702,106 @@
 3|Estrutura Dados 1|Tang
 5|Eng de Soft|Ausb||B1
 7|Metod Trab Cientif|||cct</t>
+  </si>
+  <si>
+    <t>3|Fisica II||5||C
+5|BD I|L Mariano|27|Bcct
+7|Teste Software|||Inf1</t>
+  </si>
+  <si>
+    <t>1|Prog I|Annabell|27|Bcct
+7|Metodologia|Molina
+9|Algoritmos em Grafos|L Mariano||Inf1</t>
+  </si>
+  <si>
+    <t>1|Inglês Instrumental
+10|Estágio Sup|Tang||Inf1</t>
+  </si>
+  <si>
+    <t>2|Fisica Geral I||21
+4|Sist Operacional|João|10
+6|Pesquisa Operacional|Tang|3</t>
+  </si>
+  <si>
+    <t>2|Calculo Dif e Int 2||||Eng e Comp
+4|Sis Operacional|João||BInf2
+6|Int Comp Grafica|Riv||BInf1</t>
+  </si>
+  <si>
+    <t>2|Calculo Dif e Int 2||||Eng e Comp
+4|Sis Operacional|João||BInf2
+6|Int Comp Grafica</t>
+  </si>
+  <si>
+    <t>2|Calculo Dif e Int 2||||Eng e Comp
+4|Calculo III|Oscar</t>
+  </si>
+  <si>
+    <t>2|Lógica Digital|Átila||CCT 206
+4|Cálc Numérico||||Eng e Comp
+6|Intelig Artificial|Anna||BInf1</t>
+  </si>
+  <si>
+    <t>2|Lógica Digital|Átila||CCT 206
+4|Cálc Numérico||||Eng e Comp
+6|lntelig Artificial|Anna||BInf1</t>
+  </si>
+  <si>
+    <t>3|Est Dados I CC1|Tang|16|inf2
+5|BD I|L Mariano|13|inf1
+7|Metodologia|Molina||105P3</t>
+  </si>
+  <si>
+    <t>1|Lógica Mat|Tang||AuditP5
+4|Cálc Núm|Elba||Apitão
+5|Redes de Comp|João</t>
+  </si>
+  <si>
+    <t>2|Programação 2|LM||infCCT
+9|Proj de Monografia|Riv||BInf1
+10|Estagio S|Ausb||116p5</t>
+  </si>
+  <si>
+    <t>1|Organiz Comp|Luiz M||B2
+3|Calculo III|||206 207
+5|Proc Estocást|L Guill||205 E1</t>
+  </si>
+  <si>
+    <t>3|Estrutura Dados 1|Tang||Sal 
+5|Engenharia de Soft|Ausb||B1 
+7|Metod Trab Cientif|||cct</t>
+  </si>
+  <si>
+    <t>2|Fisica 1|||106 e 109B|A e B
+6|Int Comp Grafica|Rivera||Inf2
+8|Comp Ambiental|Eduardo</t>
+  </si>
+  <si>
+    <t>1|Org Comp|Sanya|35|205_E1
+8|Empreendedorismo|||109A</t>
+  </si>
+  <si>
+    <t>1|Org Comp|Sanya|35|205_E1
+3|Est Dados I|Tang|45|106P3
+5|L Formais|Annabell|10|inf1
+7|Teste Software|João|8|inf1</t>
+  </si>
+  <si>
+    <t>2|Inglês Instrumental II||||B
+5|Comp e Socied||23|107</t>
+  </si>
+  <si>
+    <t>1|Lógica Mat|Tang|30
+3|Método Mat|Beggio|25
+2|Fisica I||||B
+3|Fisica II||||A
+3|Fisica Experimental II||||C
+7|Sistemas Distribuidos|João|6|Inf1</t>
+  </si>
+  <si>
+    <t>3|Fisica Experimental II||||A
+5|BD I|L Mariano|27|Bcct
+7|Teste Software|||Inf1</t>
   </si>
 </sst>
 </file>
@@ -993,55 +988,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1055,6 +1005,51 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1364,17 +1359,17 @@
   <dimension ref="A1:K144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12:B13"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="13.5546875" hidden="1" customWidth="1"/>
     <col min="12" max="16384" width="8.88671875" hidden="1"/>
@@ -1402,161 +1397,161 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>39</v>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>0.375</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="16" t="s">
+      <c r="B4" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>0.5</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" spans="1:6" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>40</v>
+      <c r="B8" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>0.625</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="16" t="s">
+      <c r="B10" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>5</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>0.75</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="B12" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="20"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="23"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
@@ -1764,36 +1759,36 @@
     <row r="144" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1808,23 +1803,23 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10:F11"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="8.88671875" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34"/>
+      <c r="A1" s="19"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1842,171 +1837,171 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35">
+      <c r="A2" s="20">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>147</v>
+      <c r="B2" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35">
+      <c r="A3" s="20">
         <v>0.375</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35">
+      <c r="A4" s="20">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="D4" s="26" t="s">
+      <c r="B4" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="32"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="20">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+    </row>
+    <row r="8" spans="1:6" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="20">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="20">
+        <v>0.625</v>
+      </c>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="20">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="32"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="20">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20">
+        <v>0.75</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="F5" s="26"/>
-    </row>
-    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35">
-        <v>0.5</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-    </row>
-    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-    </row>
-    <row r="8" spans="1:6" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35">
-        <v>0.625</v>
-      </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="F10" s="26"/>
-    </row>
-    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="35">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-    </row>
-    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="35">
-        <v>0.75</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="35">
+      <c r="A13" s="20">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="34"/>
+      <c r="A14" s="19"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3"/>
@@ -2014,21 +2009,11 @@
     <row r="18" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
@@ -2038,11 +2023,21 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2057,7 +2052,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C3"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -2094,205 +2089,205 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="F2" s="26"/>
+      <c r="B2" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>0.375</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>164</v>
+      <c r="B4" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>0.5</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="26"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
     </row>
     <row r="8" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>165</v>
+      <c r="B8" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>0.625</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
     </row>
     <row r="10" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>166</v>
+      <c r="B10" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>0.75</v>
       </c>
-      <c r="B12" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
+      <c r="B12" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2343,157 +2338,157 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>0.375</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>0.5</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>0.625</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>0.75</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2508,7 +2503,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12:E13"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -2543,172 +2538,172 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>55</v>
+      <c r="F2" s="28" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>0.375</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="21" t="s">
+      <c r="B4" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>56</v>
+      <c r="F4" s="28" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="17"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>0.5</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="21" t="s">
+      <c r="B8" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="28" t="s">
         <v>49</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>0.625</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
     </row>
     <row r="10" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="21" t="s">
+      <c r="B10" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="28" t="s">
         <v>50</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
     </row>
     <row r="12" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>0.75</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
     </row>
     <row r="13" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>0.79166666666666663</v>
       </c>
       <c r="B13" s="9"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="20"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="23"/>
     </row>
     <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>0.83333333333333337</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="10"/>
@@ -2716,16 +2711,16 @@
     <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
@@ -2734,16 +2729,16 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2758,7 +2753,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8:F9"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -2795,163 +2790,163 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>74</v>
+      <c r="F2" s="28" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>0.375</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>75</v>
+      <c r="B4" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
     </row>
     <row r="6" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>0.5</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
     </row>
     <row r="7" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>40</v>
+      <c r="B8" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>0.625</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
     </row>
     <row r="10" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>76</v>
+      <c r="B10" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="22"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="29"/>
     </row>
     <row r="12" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>0.75</v>
       </c>
-      <c r="B12" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="B12" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
     </row>
     <row r="13" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="20"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="23"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
@@ -2959,36 +2954,36 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3003,7 +2998,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10:F11"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -3040,171 +3035,171 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>99</v>
+      <c r="B2" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>0.375</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>89</v>
+      <c r="B4" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>150</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>98</v>
+        <v>79</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="29"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>0.5</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="18"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="25"/>
     </row>
     <row r="7" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="32"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>97</v>
+      <c r="B8" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>0.625</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
     </row>
     <row r="10" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>96</v>
+      <c r="B10" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
     </row>
     <row r="12" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>0.75</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" s="16"/>
+      <c r="B12" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="22"/>
     </row>
     <row r="13" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
@@ -3217,21 +3212,11 @@
     <row r="20" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
@@ -3240,11 +3225,21 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3259,7 +3254,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12:F13"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -3295,171 +3290,171 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>14</v>
+      <c r="E2" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>0.375</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="1:6" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>26</v>
+      <c r="B4" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>0.5</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
     </row>
     <row r="8" spans="1:6" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>22</v>
+      <c r="B8" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>0.625</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
     </row>
     <row r="10" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" s="24" t="s">
+      <c r="E10" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="F10" s="34" t="s">
         <v>17</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>0.75</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>20</v>
+      <c r="E12" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
@@ -3471,36 +3466,36 @@
     <row r="19" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3552,157 +3547,157 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>0.375</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>0.5</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>0.625</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>0.75</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3753,157 +3748,157 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>0.375</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>0.5</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>0.625</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>0.75</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3955,157 +3950,157 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>0.375</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>0.5</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>0.625</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>0.75</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4157,203 +4152,203 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>129</v>
+      <c r="B2" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>0.375</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>130</v>
+      <c r="F4" s="32" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>0.5</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
     </row>
     <row r="8" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>131</v>
+      <c r="F8" s="34" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>0.625</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
     </row>
     <row r="10" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C10" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>132</v>
+      <c r="F10" s="34" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>0.75</v>
       </c>
-      <c r="B12" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
+      <c r="B12" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
#207 Updating data in DB
</commit_message>
<xml_diff>
--- a/Files/data/Processed Data/Tabelas/CS Grids - 2019.1-2024.1.xlsx
+++ b/Files/data/Processed Data/Tabelas/CS Grids - 2019.1-2024.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\timetabling-UENF\Files\data\Processed Data\Tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8752377E-4BA1-4600-BF2A-3DDBA26FA88A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63E9B7D-378B-4D76-BA87-90C2945A75B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="704" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="10320" tabRatio="704" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="24.1-v0" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,18 @@
     <sheet name="19.1-v" sheetId="11" r:id="rId11"/>
     <sheet name="limpo" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -808,7 +819,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -880,6 +891,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -945,7 +962,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1009,11 +1026,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1021,8 +1038,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1037,19 +1054,28 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1415,11 +1441,11 @@
       <c r="A3" s="13">
         <v>0.375</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
@@ -1445,11 +1471,11 @@
       <c r="A5" s="13">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
@@ -1465,7 +1491,7 @@
       <c r="A7" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="26"/>
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
@@ -1495,11 +1521,11 @@
       <c r="A9" s="13">
         <v>0.625</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
@@ -1525,11 +1551,11 @@
       <c r="A11" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
@@ -1547,11 +1573,11 @@
       <c r="A13" s="13">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="27"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="23"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
@@ -1759,36 +1785,36 @@
     <row r="144" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1840,19 +1866,19 @@
       <c r="A2" s="20">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="34" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1860,29 +1886,29 @@
       <c r="A3" s="20">
         <v>0.375</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="32" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="34" t="s">
         <v>156</v>
       </c>
     </row>
@@ -1890,51 +1916,51 @@
       <c r="A5" s="20">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
       <c r="E5" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="F5" s="34"/>
+      <c r="F5" s="32"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20">
         <v>0.5</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
     </row>
     <row r="8" spans="1:6" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="32" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1942,63 +1968,63 @@
       <c r="A9" s="20">
         <v>0.625</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
     </row>
     <row r="10" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="32"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20">
         <v>0.75</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34" t="s">
+      <c r="C12" s="32"/>
+      <c r="D12" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19"/>
@@ -2009,21 +2035,11 @@
     <row r="18" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
@@ -2033,11 +2049,21 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2050,9 +2076,9 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10:E11"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -2089,47 +2115,47 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="F2" s="34"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>0.375</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="38"/>
       <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="33"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="37" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2138,52 +2164,52 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>0.5</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34" t="s">
+      <c r="D6" s="39"/>
+      <c r="E6" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="39"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>0.54166666666666663</v>
       </c>
       <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
     </row>
     <row r="8" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="37" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2191,29 +2217,29 @@
       <c r="A9" s="13">
         <v>0.625</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="39" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2221,35 +2247,35 @@
       <c r="A11" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>0.75</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="33"/>
       <c r="F13" s="33"/>
     </row>
@@ -2258,36 +2284,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2459,36 +2485,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2588,11 +2614,11 @@
       <c r="A5" s="13">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="23"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="29"/>
-      <c r="F5" s="23"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
@@ -2608,7 +2634,7 @@
       <c r="A7" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="26"/>
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
@@ -2670,7 +2696,7 @@
       <c r="A11" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="23"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
@@ -2695,8 +2721,8 @@
       <c r="B13" s="9"/>
       <c r="C13" s="29"/>
       <c r="D13" s="30"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="27"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="23"/>
     </row>
     <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
@@ -2711,16 +2737,16 @@
     <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
@@ -2729,16 +2755,16 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2892,7 +2918,7 @@
       </c>
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
-      <c r="D9" s="23"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
     </row>
@@ -2922,8 +2948,8 @@
       </c>
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
       <c r="F11" s="29"/>
     </row>
     <row r="12" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2943,10 +2969,10 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="B13" s="30"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="27"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="23"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
@@ -2954,36 +2980,36 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3055,11 +3081,11 @@
       <c r="A3" s="13">
         <v>0.375</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
@@ -3085,13 +3111,13 @@
       <c r="A5" s="13">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="24"/>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
@@ -3109,7 +3135,7 @@
       <c r="A7" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="31"/>
       <c r="D7" s="31"/>
       <c r="E7" s="18"/>
@@ -3139,11 +3165,11 @@
       <c r="A9" s="13">
         <v>0.625</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
     </row>
     <row r="10" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
@@ -3169,11 +3195,11 @@
       <c r="A11" s="13">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
     </row>
     <row r="12" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
@@ -3195,11 +3221,11 @@
       <c r="A13" s="13">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
@@ -3212,21 +3238,11 @@
     <row r="20" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
@@ -3235,11 +3251,21 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3290,19 +3316,19 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="34" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3320,19 +3346,19 @@
       <c r="A4" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="34" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3350,11 +3376,11 @@
       <c r="A6" s="13">
         <v>0.5</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
@@ -3370,19 +3396,19 @@
       <c r="A8" s="13">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="34" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3400,19 +3426,19 @@
       <c r="A10" s="13">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="34" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3430,19 +3456,19 @@
       <c r="A12" s="13">
         <v>0.75</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="32" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3466,36 +3492,36 @@
     <row r="19" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3547,7 +3573,7 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="35"/>
       <c r="D2" s="35"/>
       <c r="E2" s="35"/>
@@ -3668,36 +3694,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3748,7 +3774,7 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="35"/>
       <c r="D2" s="35"/>
       <c r="E2" s="35"/>
@@ -3869,36 +3895,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3950,7 +3976,7 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="35"/>
       <c r="D2" s="35"/>
       <c r="E2" s="35"/>
@@ -4071,36 +4097,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4113,9 +4139,9 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12:C13"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -4152,19 +4178,19 @@
       <c r="A2" s="13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="32" t="s">
         <v>114</v>
       </c>
     </row>
@@ -4182,19 +4208,19 @@
       <c r="A4" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="32" t="s">
         <v>115</v>
       </c>
     </row>
@@ -4212,11 +4238,11 @@
       <c r="A6" s="13">
         <v>0.5</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
@@ -4232,19 +4258,19 @@
       <c r="A8" s="13">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="34" t="s">
         <v>116</v>
       </c>
     </row>
@@ -4262,19 +4288,19 @@
       <c r="A10" s="13">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="34" t="s">
         <v>117</v>
       </c>
     </row>
@@ -4292,17 +4318,17 @@
       <c r="A12" s="13">
         <v>0.75</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
@@ -4319,36 +4345,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
#272 some file adjustments, I guess
</commit_message>
<xml_diff>
--- a/Files/data/Processed Data/Tabelas/CS Grids - 2019.1-2024.1.xlsx
+++ b/Files/data/Processed Data/Tabelas/CS Grids - 2019.1-2024.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\timetabling-UENF\Files\data\Processed Data\Tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63E9B7D-378B-4D76-BA87-90C2945A75B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A7E260-7059-4265-896A-0816F8912E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="10320" tabRatio="704" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="10320" tabRatio="704" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="24.1-v0" sheetId="1" r:id="rId1"/>
@@ -819,7 +819,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -897,6 +897,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -962,14 +975,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -999,9 +1009,6 @@
     <xf numFmtId="20" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1026,11 +1033,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1038,8 +1045,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1054,13 +1061,13 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1076,6 +1083,18 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1392,7 +1411,7 @@
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="34" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.5546875" bestFit="1" customWidth="1"/>
@@ -1402,8 +1421,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1420,273 +1439,273 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="20" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>0.375</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>0.5</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
     </row>
     <row r="8" spans="1:6" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="20" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>0.625</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="20" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="A12" s="12">
         <v>0.75</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="12">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="23"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="25"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="C14" s="11"/>
+      <c r="A14" s="11"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="11"/>
+      <c r="C15" s="10"/>
     </row>
     <row r="16" spans="1:6" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="11"/>
+      <c r="C16" s="10"/>
     </row>
     <row r="17" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="11"/>
+      <c r="C17" s="10"/>
     </row>
     <row r="18" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="11"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="11"/>
+      <c r="C19" s="10"/>
     </row>
     <row r="20" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="11"/>
+      <c r="C20" s="10"/>
     </row>
     <row r="21" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="11"/>
+      <c r="C21" s="10"/>
     </row>
     <row r="22" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="11"/>
+      <c r="C22" s="10"/>
     </row>
     <row r="23" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="11"/>
+      <c r="C23" s="10"/>
     </row>
     <row r="24" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="11"/>
+      <c r="C24" s="10"/>
     </row>
     <row r="25" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="11"/>
+      <c r="C25" s="10"/>
     </row>
     <row r="26" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="11"/>
+      <c r="C26" s="10"/>
     </row>
     <row r="27" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="11"/>
+      <c r="C27" s="10"/>
     </row>
     <row r="28" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="11"/>
+      <c r="C28" s="10"/>
     </row>
     <row r="29" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="11"/>
+      <c r="C29" s="10"/>
     </row>
     <row r="30" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="11"/>
+      <c r="C30" s="10"/>
     </row>
     <row r="31" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="11"/>
+      <c r="C31" s="10"/>
     </row>
     <row r="32" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="11"/>
+      <c r="C32" s="10"/>
     </row>
     <row r="33" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="11"/>
+      <c r="C33" s="10"/>
     </row>
     <row r="34" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="11"/>
+      <c r="C34" s="10"/>
     </row>
     <row r="35" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="11"/>
+      <c r="C35" s="10"/>
     </row>
     <row r="36" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="11"/>
+      <c r="C36" s="10"/>
     </row>
     <row r="37" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="11"/>
+      <c r="C37" s="10"/>
     </row>
     <row r="38" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="11"/>
+      <c r="C38" s="10"/>
     </row>
     <row r="39" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="11"/>
+      <c r="C39" s="10"/>
     </row>
     <row r="40" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="11"/>
+      <c r="C40" s="10"/>
     </row>
     <row r="41" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="11"/>
+      <c r="C41" s="10"/>
     </row>
     <row r="42" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="11"/>
+      <c r="C42" s="10"/>
     </row>
     <row r="43" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="11"/>
+      <c r="C43" s="10"/>
     </row>
     <row r="44" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="11"/>
+      <c r="C44" s="10"/>
     </row>
     <row r="45" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="11"/>
+      <c r="C45" s="10"/>
     </row>
     <row r="46" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="11"/>
+      <c r="C46" s="10"/>
     </row>
     <row r="47" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="11"/>
+      <c r="C47" s="10"/>
     </row>
     <row r="48" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="11"/>
+      <c r="C48" s="10"/>
     </row>
     <row r="49" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="11"/>
+      <c r="C49" s="10"/>
     </row>
     <row r="50" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="3:3" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1785,36 +1804,36 @@
     <row r="144" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1827,14 +1846,14 @@
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10:D11"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.109375" bestFit="1" customWidth="1"/>
@@ -1845,7 +1864,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19"/>
+      <c r="A1" s="17"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1863,171 +1882,171 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20">
+      <c r="A2" s="18">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="39" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20">
+      <c r="A3" s="18">
         <v>0.375</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20">
+      <c r="A4" s="18">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="39" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20">
+      <c r="A5" s="18">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="14" t="s">
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="38"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20">
+      <c r="A6" s="18">
         <v>0.5</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20">
+      <c r="A7" s="18">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
     </row>
     <row r="8" spans="1:6" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20">
+      <c r="A8" s="18">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="38" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20">
+      <c r="A9" s="18">
         <v>0.625</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20">
+      <c r="A10" s="18">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="F10" s="32"/>
+      <c r="F10" s="38"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20">
+      <c r="A11" s="18">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20">
+      <c r="A12" s="18">
         <v>0.75</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32" t="s">
+      <c r="C12" s="38"/>
+      <c r="D12" s="38" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="32"/>
       <c r="F12" s="32"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20">
+      <c r="A13" s="18">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="32"/>
       <c r="F13" s="32"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
+      <c r="A14" s="17"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3"/>
@@ -2035,11 +2054,21 @@
     <row r="18" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
@@ -2049,21 +2078,11 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2076,7 +2095,7 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C4" sqref="C4:C5"/>
     </sheetView>
@@ -2094,7 +2113,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
+      <c r="A1" s="11"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2112,208 +2131,208 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="35" t="s">
         <v>157</v>
       </c>
       <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>0.375</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="33"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="35" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>0.5</v>
       </c>
       <c r="B6" s="32"/>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39" t="s">
+      <c r="D6" s="37"/>
+      <c r="E6" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="37"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="35" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>0.625</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="35" t="s">
         <v>140</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="37" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="A12" s="12">
         <v>0.75</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="37" t="s">
         <v>110</v>
       </c>
       <c r="E12" s="32"/>
       <c r="F12" s="32"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="12">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2343,7 +2362,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
+      <c r="A1" s="11"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2361,160 +2380,160 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>0.375</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>0.5</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>0.625</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="A12" s="12">
         <v>0.75</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="12">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2537,13 +2556,13 @@
     <col min="1" max="1" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="30.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
+      <c r="A1" s="11"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2556,197 +2575,197 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="26" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>0.375</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="26" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="24"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>0.5</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="7"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="6" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="26" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>0.625</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
     </row>
     <row r="10" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="26" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
     </row>
     <row r="12" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="A12" s="12">
         <v>0.75</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="12">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="23"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="25"/>
     </row>
     <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13">
+      <c r="A14" s="12">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="10"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
@@ -2755,16 +2774,16 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2785,7 +2804,7 @@
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.109375" bestFit="1" customWidth="1"/>
@@ -2795,8 +2814,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -2813,203 +2832,203 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="26" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>0.375</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="26" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>0.5</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
     </row>
     <row r="8" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="26" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>0.625</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
     </row>
     <row r="10" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="26" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="29"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="27"/>
     </row>
     <row r="12" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="A12" s="12">
         <v>0.75</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="12">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="23"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="25"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="11"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3030,7 +3049,7 @@
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.88671875" bestFit="1" customWidth="1"/>
@@ -3040,8 +3059,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -3058,177 +3077,177 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="20" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>0.375</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="20" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="16" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="27"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>0.5</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="17" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="23"/>
     </row>
     <row r="7" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="31"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="29"/>
     </row>
     <row r="8" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="20" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>0.625</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="20" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="A12" s="12">
         <v>0.75</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22" t="s">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="22"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="12">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="11"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3"/>
@@ -3238,11 +3257,21 @@
     <row r="20" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
@@ -3251,21 +3280,11 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3295,7 +3314,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
+      <c r="A1" s="11"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3313,67 +3332,67 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="30" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>0.375</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="30" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>0.5</v>
       </c>
       <c r="B6" s="32"/>
@@ -3383,77 +3402,77 @@
       <c r="F6" s="32"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:6" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="30" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>0.625</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
     </row>
     <row r="10" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="A12" s="12">
         <v>0.75</v>
       </c>
       <c r="B12" s="32" t="s">
@@ -3473,17 +3492,17 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="12">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="11"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3"/>
@@ -3492,36 +3511,36 @@
     <row r="19" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3552,7 +3571,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
+      <c r="A1" s="11"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3570,160 +3589,160 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>0.375</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>0.5</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>0.625</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="A12" s="12">
         <v>0.75</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="12">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3753,7 +3772,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
+      <c r="A1" s="11"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3771,160 +3790,160 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>0.375</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>0.5</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>0.625</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="A12" s="12">
         <v>0.75</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="12">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3955,7 +3974,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
+      <c r="A1" s="11"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3973,160 +3992,160 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>0.375</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>0.5</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>0.625</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="A12" s="12">
         <v>0.75</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="12">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4157,7 +4176,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
+      <c r="A1" s="11"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4175,19 +4194,19 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="30" t="s">
         <v>102</v>
       </c>
       <c r="F2" s="32" t="s">
@@ -4195,29 +4214,29 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+      <c r="A3" s="12">
         <v>0.375</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="12">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="30" t="s">
         <v>111</v>
       </c>
       <c r="F4" s="32" t="s">
@@ -4225,17 +4244,17 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="12">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>0.5</v>
       </c>
       <c r="B6" s="32"/>
@@ -4245,77 +4264,77 @@
       <c r="F6" s="32"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7" s="12">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+      <c r="A8" s="12">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="30" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+      <c r="A9" s="12">
         <v>0.625</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
     </row>
     <row r="10" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="30" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
+      <c r="A12" s="12">
         <v>0.75</v>
       </c>
       <c r="B12" s="32" t="s">
@@ -4331,50 +4350,50 @@
       <c r="F12" s="32"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="12">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>